<commit_message>
update MinioService, download excel template
</commit_message>
<xml_diff>
--- a/Services/TenantManagement/SeedData/student_upload.xlsx
+++ b/Services/TenantManagement/SeedData/student_upload.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Danh sách sinh viên</t>
   </si>
@@ -60,24 +60,6 @@
   </si>
   <si>
     <t>Số điện thoại</t>
-  </si>
-  <si>
-    <t>Trần Văn A</t>
-  </si>
-  <si>
-    <t>KH001</t>
-  </si>
-  <si>
-    <t>Công nghệ thông tin</t>
-  </si>
-  <si>
-    <t>K64CCLC</t>
-  </si>
-  <si>
-    <t>19020060@vnu.edu.vn</t>
-  </si>
-  <si>
-    <t>0348200145</t>
   </si>
 </sst>
 </file>
@@ -739,9 +721,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1280,7 +1259,7 @@
   <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1342,37 +1321,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>19020001</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1">
-        <v>3.6</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>16</v>
-      </c>
+    <row r="4" spans="9:9">
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="9:9">
       <c r="I5" s="5"/>
@@ -1693,9 +1643,6 @@
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1" display="19020060@vnu.edu.vn" tooltip="mailto:19020060@vnu.edu.vn"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
cap nhat file upload
</commit_message>
<xml_diff>
--- a/Services/TenantManagement/SeedData/student_upload.xlsx
+++ b/Services/TenantManagement/SeedData/student_upload.xlsx
@@ -1256,14 +1256,14 @@
   <dimension ref="A1:I109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.42857142857143" customWidth="1"/>
     <col min="2" max="2" width="19.8571428571429" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="14.2857142857143" customWidth="1"/>
     <col min="5" max="5" width="26.8571428571429" customWidth="1"/>
     <col min="7" max="7" width="9.14285714285714" style="1"/>

</xml_diff>